<commit_message>
feat: Add authentication service, implement granular permissions for module access, and introduce a new preparation module.
</commit_message>
<xml_diff>
--- a/public/template_preparacao.xlsx
+++ b/public/template_preparacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafae\OneDrive\Documentos\TECPLAM-MAR\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8C0864-68CC-418A-9518-34CF750274CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C305BF1-CEC9-4C9C-B926-5457E8FDE070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2124" yWindow="2124" windowWidth="15600" windowHeight="9972" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -763,7 +763,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -855,16 +855,7 @@
     <xf numFmtId="164" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -995,6 +986,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1460,7 +1463,7 @@
   <dimension ref="B1:AA7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E2" sqref="E2:R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1477,122 +1480,122 @@
   <sheetData>
     <row r="1" spans="2:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="45" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="36" t="s">
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="38"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="35"/>
     </row>
     <row r="3" spans="2:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="39" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="40"/>
-      <c r="U3" s="40"/>
-      <c r="V3" s="41"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="38"/>
     </row>
     <row r="4" spans="2:27" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="52"/>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="52"/>
-      <c r="R4" s="53"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="44"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="41"/>
     </row>
     <row r="5" spans="2:27" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:27" s="1" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
       <c r="Q6" s="30"/>
       <c r="R6" s="30"/>
       <c r="S6" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="T6" s="34">
+      <c r="T6" s="77">
         <f ca="1">TODAY()</f>
         <v>46069</v>
       </c>
-      <c r="U6" s="34"/>
-      <c r="V6" s="34"/>
+      <c r="U6" s="77"/>
+      <c r="V6" s="77"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
     </row>
     <row r="7" spans="2:27" s="1" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="26" t="s">
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="27" t="s">
@@ -1637,13 +1640,13 @@
       <c r="S7" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="T7" s="31" t="s">
+      <c r="T7" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="U7" s="31" t="s">
+      <c r="U7" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="V7" s="31" t="s">
+      <c r="V7" s="78" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1685,32 +1688,32 @@
     <row r="5" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="18"/>
       <c r="C5" s="19"/>
-      <c r="D5" s="65" t="s">
+      <c r="D5" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="55" t="s">
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="52" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="20"/>
       <c r="C6" s="21"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="56"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="53"/>
     </row>
     <row r="7" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="20"/>
       <c r="C7" s="21"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
       <c r="H7" s="22" t="s">
         <v>26</v>
       </c>
@@ -1718,24 +1721,24 @@
     <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="20"/>
       <c r="C8" s="21"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
       <c r="H8" s="29"/>
     </row>
     <row r="9" spans="2:8" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="70"/>
+      <c r="C9" s="67"/>
       <c r="D9" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="71" t="s">
+      <c r="E9" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="70"/>
+      <c r="F9" s="67"/>
       <c r="G9" s="24" t="s">
         <v>14</v>
       </c>
@@ -1744,17 +1747,17 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="72">
+      <c r="B10" s="69">
         <v>44980</v>
       </c>
-      <c r="C10" s="73"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="74" t="s">
+      <c r="E10" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="75"/>
+      <c r="F10" s="72"/>
       <c r="G10" s="4" t="s">
         <v>19</v>
       </c>
@@ -1763,17 +1766,17 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="72">
+      <c r="B11" s="69">
         <v>45337</v>
       </c>
-      <c r="C11" s="73"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="76" t="s">
+      <c r="E11" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="77"/>
+      <c r="F11" s="74"/>
       <c r="G11" s="7" t="s">
         <v>27</v>
       </c>
@@ -1818,20 +1821,20 @@
       <c r="H15" s="14"/>
     </row>
     <row r="16" spans="2:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="57"/>
-      <c r="C16" s="58"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="60"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
       <c r="G16" s="12"/>
       <c r="H16" s="14"/>
     </row>
     <row r="17" spans="2:8" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="61"/>
-      <c r="C17" s="62"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="59"/>
       <c r="D17" s="15"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="64"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="61"/>
       <c r="G17" s="16"/>
       <c r="H17" s="17"/>
     </row>

</xml_diff>